<commit_message>
Fixed and added the results for the likelihood plot
</commit_message>
<xml_diff>
--- a/graphs/periodicRunnings.xlsx
+++ b/graphs/periodicRunnings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="463" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="463" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="periodic_10" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="20">
   <si>
     <t>Periodic Data – p =.998 q = .70</t>
   </si>
@@ -158,7 +158,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -171,8 +171,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Periodic 10</a:t>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Periodicity 10</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -190,7 +190,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -873,7 +873,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -912,7 +911,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -925,7 +924,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Avg Block Size</a:t>
                 </a:r>
               </a:p>
@@ -944,7 +943,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -982,7 +981,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1029,7 +1028,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1042,7 +1041,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="1"/>
                   <a:t>Ratio</a:t>
                 </a:r>
               </a:p>
@@ -1061,7 +1060,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1099,7 +1098,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1141,7 +1140,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1228,8 +1227,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Periodicity</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Periodic 15</a:t>
+              <a:t> 15</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2285,7 +2290,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Periodic 20</a:t>
+              <a:t>Periodicity 20</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2490,501 +2495,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>periodic_10!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Winnowing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>periodic_20!$E$6:$E$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>5.7441108895681303</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5204905528128592</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.182430844022399</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19.465203955876401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19.655731907068098</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19.834323809149801</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20.269702040172501</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20.3427813268911</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20.4154796887195</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20.489153905746701</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20.568161644204299</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20.640637943218199</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20.7136172195464</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.787565331074202</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>20.861960924576699</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>20.9358155883492</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>21.010330396538698</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>21.0858772313385</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>21.161715928282199</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>periodic_20!$F$6:$F$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0.96316640899999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.95555422700000003</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.94047997299999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.93924454499999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.93658622000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.93310640700000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.92892862499999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.92562182100000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.92233524499999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.91904303399999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.91575336900000004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.912517778</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.90930150099999996</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.90607865399999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.90286736499999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.89970689199999998</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.89655777599999997</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.89340206899999997</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.89025996799999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6245-411A-8E60-7788715AF061}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>periodic_15!$J$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TDDD</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>periodic_20!$M$6:$M$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>24.2649345663676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57.349204660667901</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>67.2250808727444</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>119.641226819978</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>138.96770138397801</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>186.19810302008199</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>176.059433314366</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>247.01457749281099</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>288.50548618320403</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>320.71258457944901</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>334.84569373704198</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>401.57549553695202</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>418.73170696010402</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>492.51072570597898</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>463.48417536458498</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>527.64994992456297</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>580.25214968444402</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>641.90030706003495</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>634.22298014026001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>periodic_20!$N$6:$N$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0.52465583900000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.77125564499999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.66478425600000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.62643299900000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.58380656399999997</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.52768027399999995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.52251231799999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.46850050300000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.37336813000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.34729222500000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.36674891199999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.279242451</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.267654479</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.20129681899999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.26339364100000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.197914534</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.189186191</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.142628159</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.16877724099999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6245-411A-8E60-7788715AF061}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>periodic_10!$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2min</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="7030A0"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>periodic_20!$H$6:$H$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>20.0493457045017</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.384381984160299</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3592.51098605579</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3809.85623270118</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3917.35996218322</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3924.89701026274</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10851.285606720499</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10855.906955840899</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10860.761668195501</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10865.663674109601</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11109.3433486003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11114.2832862215</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11119.138648587599</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>11123.667148570399</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>11128.5879310377</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11133.2819273607</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11138.445815274399</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11144.320914349901</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11150.4644929061</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>periodic_20!$I$6:$I$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0.93292006199999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.92601277900000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6245-411A-8E60-7788715AF061}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2995,6 +2505,565 @@
         </c:dLbls>
         <c:axId val="411149832"/>
         <c:axId val="411150160"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_10!$D$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Winnowing</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="31750" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="00B050"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$E$6:$E$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>5.7441108895681303</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8.5204905528128592</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>19.182430844022399</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>19.465203955876401</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>19.655731907068098</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>19.834323809149801</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>20.269702040172501</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>20.3427813268911</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>20.4154796887195</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>20.489153905746701</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>20.568161644204299</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>20.640637943218199</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>20.7136172195464</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>20.787565331074202</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>20.861960924576699</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>20.9358155883492</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>21.010330396538698</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>21.0858772313385</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>21.161715928282199</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$F$6:$F$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>0.96316640899999995</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.95555422700000003</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.94047997299999997</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.93924454499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.93658622000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.93310640700000003</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.92892862499999995</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.92562182100000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.92233524499999997</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.91904303399999998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.91575336900000004</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.912517778</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.90930150099999996</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.90607865399999998</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.90286736499999998</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.89970689199999998</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.89655777599999997</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.89340206899999997</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.89025996799999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-6245-411A-8E60-7788715AF061}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_15!$J$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>TDDD</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="FF0000"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$M$6:$M$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>24.2649345663676</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>57.349204660667901</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>67.2250808727444</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>119.641226819978</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>138.96770138397801</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>186.19810302008199</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>176.059433314366</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>247.01457749281099</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>288.50548618320403</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>320.71258457944901</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>334.84569373704198</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>401.57549553695202</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>418.73170696010402</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>492.51072570597898</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>463.48417536458498</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>527.64994992456297</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>580.25214968444402</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>641.90030706003495</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>634.22298014026001</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$N$6:$N$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>0.52465583900000001</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.77125564499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.66478425600000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.62643299900000005</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.58380656399999997</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.52768027399999995</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.52251231799999998</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.46850050300000001</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.37336813000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.34729222500000001</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.36674891199999998</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.279242451</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.267654479</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.20129681899999999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.26339364100000001</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.197914534</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.189186191</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.142628159</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.16877724099999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-6245-411A-8E60-7788715AF061}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_10!$G$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>2min</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:solidFill>
+                      <a:srgbClr val="7030A0"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$H$6:$H$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>20.0493457045017</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>20.384381984160299</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3592.51098605579</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3809.85623270118</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3917.35996218322</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3924.89701026274</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>10851.285606720499</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>10855.906955840899</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>10860.761668195501</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>10865.663674109601</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>11109.3433486003</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>11114.2832862215</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>11119.138648587599</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>11123.667148570399</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>11128.5879310377</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>11133.2819273607</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>11138.445815274399</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>11144.320914349901</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>11150.4644929061</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>periodic_20!$I$6:$I$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="19"/>
+                      <c:pt idx="0">
+                        <c:v>0.93292006199999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.92601277900000001</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-6245-411A-8E60-7788715AF061}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="411149832"/>
@@ -3341,7 +3410,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Periodic 25</a:t>
+              <a:t>Periodicity 25</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5418,6 +5487,785 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>periodic_30!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TDDD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>periodic_30!$M$6:$M$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>32.273972606964897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.905459060999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84.458262087458294</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.634064122108697</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121.96485264406</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>158.275528581418</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>199.42233007198101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>215.93521612783201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>269.130850623664</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>297.53067872624001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>341.79068574256701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>356.62807537170301</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>388.79205407495198</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>381.335242898839</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>473.98394942104801</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>511.516453155433</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>529.77642220924497</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>537.19519819751201</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>614.75957575220605</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>periodic_30!$N$6:$N$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.81687765324469297</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52552459495081005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.77168063563872902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73488975022049896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57475579348841299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66497130305739405</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56444796310407397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47564685970628101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47299726500547001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.43417702964594102</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33144181811636397</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.37881013237973499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.36431058837882302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.36117455365089302</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29428456543086901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.27261494577010797</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.23491478417043199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.28705999388001202</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20310791878416201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FFA1-4F62-BFE2-FD13554266C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2min - relaxed</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>periodic_30!$P$6:$P$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>23.017036171683301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.049741102168799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.4261629526493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.7593300984127</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60.098056105383797</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.428265630162997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.761284192119497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61.095588205311202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.426154338518799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.760473273877501</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90.684388390943795</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91.165156892710897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>91.650488501358595</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92.134648307332398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>92.629810035766397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>93.1314466330154</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>121.76842867481901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>122.412321548557</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>123.058991340367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>periodic_30!$Q$6:$Q$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.92692878014243996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91116770666458602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90617659064681799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90102125995747995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8581542996914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85348476203047596</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84886470327059305</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84419577160845705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.83973753052493905</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83530722738554497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79145266809466397</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.78725026549946897</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.78306565186869603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.77898153303693396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.77486950726098602</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.77071676256647503</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.72906226387547202</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.72524002751994499</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.72145663108673797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FFA1-4F62-BFE2-FD13554266C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>periodic_30!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>periodic_30!$B$6:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>37.815627535069801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.018999385505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>284.70431662568802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>291.93134424316202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>484.51882756509099</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>620.62326506143995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>926.50077201354497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>980.83417660183602</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1282.0963192009301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1474.66075994994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1738.9496043090901</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1734.10166464808</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1954.54077067714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1819.2581373334999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2446.4965971902898</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2709.1544262041398</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2787.1323277699898</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2694.8430028000098</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3321.4888753998398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>periodic_30!$C$6:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.88872176455647001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78844188411623195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63453717092565798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68888708722582603</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.58474703250593496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54637836524326899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.42673854252291499</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45351172897654202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.37074016351967298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34201638196723599</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.29620048059903897</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.34202255495488998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.31335275129449702</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39746387807224398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25882697434605101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.23088569522860899</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.24896016707966601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.30432905934188098</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.203326518346963</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FFA1-4F62-BFE2-FD13554266C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="415050448"/>
+        <c:axId val="415051760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="415050448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="300"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="415051760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="415051760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="415050448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5618,6 +6466,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7683,6 +8571,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8238,15 +9642,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>224116</xdr:colOff>
+      <xdr:colOff>224115</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>156881</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>64995</xdr:rowOff>
+      <xdr:colOff>549087</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8373,6 +9777,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>694764</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>29136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>627529</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>105336</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8680,8 +10114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8727,6 +10161,9 @@
       <c r="J4" t="s">
         <v>6</v>
       </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
       <c r="O4" t="s">
         <v>5</v>
       </c>
@@ -9695,8 +11132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="G24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9886,7 +11323,7 @@
         <v>15</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:L24" si="0">FLOOR( J7/2,1) + 1</f>
+        <f t="shared" ref="K7:K24" si="0">FLOOR( J7/2,1) + 1</f>
         <v>8</v>
       </c>
       <c r="L7">
@@ -10859,8 +12296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11871,8 +13308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12883,8 +14320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>